<commit_message>
Updated scripts for processing data and joining choice data with self-report data
</commit_message>
<xml_diff>
--- a/01_data/02_processed/ChoiceData_dictionary.xlsx
+++ b/01_data/02_processed/ChoiceData_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\My-Linh\Dropbox\University of Melbourne\Dissertation\CH 5 BWDCE\jubilant-journey\01_data\02_processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3082F83-4378-4DAF-87C8-3DAE9BF111B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17099A3E-0B58-4E32-8FBE-06868F6F97C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D6F4789F-FD74-4B47-8827-BC5D72AE9A2D}"/>
+    <workbookView xWindow="-27570" yWindow="3930" windowWidth="14400" windowHeight="7365" xr2:uid="{D6F4789F-FD74-4B47-8827-BC5D72AE9A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -327,9 +327,6 @@
     <t>Yes No</t>
   </si>
   <si>
-    <t>Female, Male, Other, Prefer not to answer</t>
-  </si>
-  <si>
     <t>0-10</t>
   </si>
   <si>
@@ -340,6 +337,9 @@
   </si>
   <si>
     <t>Western Australia, Northern Territory, South Australia, Queensland, New South Wales, Victoria, Tasmania, Australian Capital Territory, Prefer not to say</t>
+  </si>
+  <si>
+    <t>1= Male, 2= Female</t>
   </si>
 </sst>
 </file>
@@ -719,7 +719,7 @@
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1002,7 +1002,7 @@
         <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -1013,7 +1013,7 @@
         <v>75</v>
       </c>
       <c r="C32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -1024,7 +1024,7 @@
         <v>76</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -1035,7 +1035,7 @@
         <v>77</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -1046,7 +1046,7 @@
         <v>78</v>
       </c>
       <c r="C35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1065,7 +1065,7 @@
         <v>43</v>
       </c>
       <c r="C37" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -1117,7 +1117,7 @@
         <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>